<commit_message>
noanom rafael ano > noanon et nosej integer mco
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RAFAEL ANO 12.xlsx
+++ b/formats/excel/Formats RAFAEL ANO 12.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24120" windowHeight="12855"/>
+    <workbookView windowWidth="24240" windowHeight="12855"/>
   </bookViews>
   <sheets>
     <sheet name="ANO-ACE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ANO-ACE'!$A$1:$F$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ANO-ACE'!$A$1:$F$12</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -79,7 +79,7 @@
     <t>N° Anonyme du patient</t>
   </si>
   <si>
-    <t>NOANOM</t>
+    <t>NOANON</t>
   </si>
   <si>
     <t>N° de séjour</t>
@@ -114,8 +114,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -132,7 +132,90 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -140,8 +223,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,6 +247,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,122 +275,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -292,85 +292,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,97 +472,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,17 +486,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -566,11 +560,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -586,148 +586,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1097,7 +1097,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="$A11:$XFD12"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="5"/>
@@ -1351,7 +1351,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F10"/>
+  <autoFilter ref="A1:F12"/>
   <pageMargins left="0.786805555555556" right="0.786805555555556" top="0.984027777777778" bottom="0.984027777777778" header="0.491666666666667" footer="0.491666666666667"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>